<commit_message>
Katalon project had to be manually rebased to avoid merge conflicts
</commit_message>
<xml_diff>
--- a/COMP72070_Section3_Group1/ClientLogs.xlsx
+++ b/COMP72070_Section3_Group1/ClientLogs.xlsx
@@ -36,7 +36,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:si>
+    <x:t>2024 April 06 4:16:05 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ASP_SERVER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Packet sent. Type: ReadyImage</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2024 April 06 4:16:10 AM</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TCP_SERVER</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Images received. Count: 6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Packet sent. Type: ReadyPost</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Posts received. Count: 4</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,18 +430,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5905D49F-3DC1-4DB0-85C3-5B62E5C53D1D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A186" zoomScale="216" workbookViewId="0">
-      <selection activeCell="C193" sqref="A1:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{5905D49F-3DC1-4DB0-85C3-5B62E5C53D1D}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" topLeftCell="A186" zoomScale="216" workbookViewId="0">
+      <x:selection activeCell="C193" sqref="A1:XFD1048576"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1">
+      <x:c r="A1" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" t="s">
+        <x:v>2</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2">
+      <x:c r="A2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" t="s">
+        <x:v>5</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3">
+      <x:c r="A3" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B3" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4">
+      <x:c r="A4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C4" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</x:worksheet>
 </file>
</xml_diff>